<commit_message>
add a testcase to skill feature
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kelly\Mars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC967826-40BA-4281-A563-AA6E3AB915D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3474D7D3-BB73-47C4-88D3-DF4EE4CBAB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="0" windowWidth="27690" windowHeight="15480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use_Stories" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="215">
   <si>
     <t>Test Scenario_ID</t>
   </si>
@@ -766,6 +766,22 @@
 3. edit the language with a non-existing lanagate
 4. click [Cancel] button
 </t>
+  </si>
+  <si>
+    <t>create a new skill with empty value</t>
+  </si>
+  <si>
+    <t>1. navigate to the profile -&gt;skill page;
+2.click the [Add New] button;
+3. Leave skill is empty, select a level or enter a language, not select level
+4. click[Cancel] button</t>
+  </si>
+  <si>
+    <t>Null, Expert
+java ,Null</t>
+  </si>
+  <si>
+    <t>display message:Please enter skill and level</t>
   </si>
 </sst>
 </file>
@@ -853,7 +869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -887,7 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1128,7 +1143,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1233,41 +1248,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O995"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="34" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="18" customWidth="1"/>
-    <col min="8" max="8" width="46" style="18" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="18" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="18" customWidth="1"/>
-    <col min="15" max="27" width="8.5703125" style="18" customWidth="1"/>
-    <col min="28" max="16384" width="12.5703125" style="18"/>
+    <col min="1" max="1" width="33.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="34" style="17" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="46" style="17" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="17" customWidth="1"/>
+    <col min="15" max="27" width="8.5703125" style="17" customWidth="1"/>
+    <col min="28" max="16384" width="12.5703125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -1282,25 +1297,25 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1308,13 +1323,13 @@
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>141</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1327,29 +1342,29 @@
       <c r="H2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="17"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1365,7 +1380,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="15" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -1374,18 +1389,18 @@
       <c r="J3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="4" t="s">
         <v>123</v>
       </c>
@@ -1396,27 +1411,27 @@
         <v>143</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="15" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
@@ -1427,28 +1442,28 @@
         <v>136</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="15" t="s">
         <v>204</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="4" t="s">
         <v>125</v>
       </c>
@@ -1462,7 +1477,7 @@
         <v>142</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>102</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -1471,19 +1486,19 @@
       <c r="J6" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="4" t="s">
         <v>126</v>
       </c>
@@ -1497,7 +1512,7 @@
         <v>142</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="15" t="s">
         <v>152</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -1506,13 +1521,13 @@
       <c r="J7" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1520,7 +1535,7 @@
       <c r="C8" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>156</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1529,29 +1544,29 @@
       <c r="F8" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="21" t="s">
+      <c r="M8" s="18"/>
+      <c r="N8" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="17"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="4" t="s">
         <v>130</v>
       </c>
@@ -1563,22 +1578,22 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>73</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1586,29 +1601,29 @@
       <c r="C10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>137</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="15" t="s">
         <v>74</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1616,7 +1631,7 @@
       <c r="A11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>160</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1639,13 +1654,13 @@
       <c r="J11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1678,13 +1693,13 @@
       <c r="J12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1692,7 +1707,7 @@
       <c r="A13" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1717,13 +1732,13 @@
       <c r="J13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="19" t="s">
+      <c r="N13" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1751,19 +1766,19 @@
       <c r="J14" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="20" t="s">
+      <c r="N14" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="17"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
         <v>157</v>
       </c>
@@ -1789,10 +1804,10 @@
       <c r="K15" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1825,13 +1840,13 @@
       <c r="J16" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="N16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4798,43 +4813,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4222C0-246C-4482-83FC-C51BDBD8EC83}">
-  <dimension ref="A1:O993"/>
+  <dimension ref="A1:O994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="34" style="18" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="18" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="18" customWidth="1"/>
-    <col min="15" max="27" width="8.5703125" style="18" customWidth="1"/>
-    <col min="28" max="16384" width="12.5703125" style="18"/>
+    <col min="1" max="1" width="15.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="34" style="17" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="17" customWidth="1"/>
+    <col min="15" max="27" width="8.5703125" style="17" customWidth="1"/>
+    <col min="28" max="16384" width="12.5703125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -4849,39 +4864,39 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>208</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -4894,29 +4909,29 @@
       <c r="H2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="17"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -4932,7 +4947,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="15" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -4941,18 +4956,18 @@
       <c r="J3" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="4" t="s">
         <v>123</v>
       </c>
@@ -4963,66 +4978,64 @@
         <v>136</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="15" t="s">
         <v>46</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
+    <row r="5" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="18"/>
       <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="16" t="s">
-        <v>47</v>
+      <c r="F5" s="4"/>
+      <c r="H5" s="15" t="s">
+        <v>212</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="L5" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>185</v>
+        <v>124</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>136</v>
@@ -5030,139 +5043,133 @@
       <c r="F6" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="15" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="L6" s="17" t="s">
+      <c r="J6" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="20" t="s">
-        <v>43</v>
+      <c r="N6" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>67</v>
+        <v>125</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>185</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="H7" s="16" t="s">
-        <v>69</v>
+      <c r="F7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="L7" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>29</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>68</v>
+        <v>126</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="16" t="s">
-        <v>70</v>
+      <c r="H8" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
+    <row r="9" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>127</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>48</v>
+      <c r="H9" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="L9" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>24</v>
+    <row r="10" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>136</v>
@@ -5172,32 +5179,36 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>190</v>
+        <v>48</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="L10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>136</v>
@@ -5207,31 +5218,32 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
-        <v>61</v>
+        <v>190</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>193</v>
+        <v>52</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>136</v>
@@ -5241,51 +5253,50 @@
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>195</v>
+        <v>192</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>193</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N12" s="20" t="s">
-        <v>43</v>
+      <c r="N12" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="17"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>196</v>
+        <v>65</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>197</v>
+        <v>194</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>29</v>
@@ -5294,55 +5305,79 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>57</v>
-      </c>
+    <row r="14" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>170</v>
+        <v>39</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="N14" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C16" s="4"/>
@@ -5355,52 +5390,60 @@
       <c r="J16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.2">
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.2">
@@ -8285,6 +8328,9 @@
     </row>
     <row r="993" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F993" s="4"/>
+    </row>
+    <row r="994" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F994" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -8401,8 +8447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07BB5CA-8C78-4318-BAD0-57AA013370E9}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8460,7 +8506,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -8468,7 +8514,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B8" s="13" t="s">

</xml_diff>

<commit_message>
optimize the language and skill feature, add the FeatureContect to implement conditional login logic
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kelly\Mars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3474D7D3-BB73-47C4-88D3-DF4EE4CBAB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC7F7FE-271D-49DE-9358-D2A49F18B49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use_Stories" sheetId="2" r:id="rId1"/>
@@ -869,7 +869,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -919,6 +919,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1248,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1323,7 +1326,7 @@
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1364,7 +1367,7 @@
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1404,7 +1407,7 @@
       <c r="C4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="21" t="s">
         <v>139</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1435,7 +1438,7 @@
       <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="21" t="s">
         <v>203</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1467,7 +1470,7 @@
       <c r="C6" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="21" t="s">
         <v>151</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1502,7 +1505,7 @@
       <c r="C7" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="21" t="s">
         <v>150</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1535,7 +1538,7 @@
       <c r="C8" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="19" t="s">
         <v>156</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1570,7 +1573,7 @@
       <c r="C9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="21" t="s">
         <v>138</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1601,7 +1604,7 @@
       <c r="C10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="19" t="s">
         <v>137</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -4815,8 +4818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4222C0-246C-4482-83FC-C51BDBD8EC83}">
   <dimension ref="A1:O994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4937,7 +4940,7 @@
       <c r="C3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -4971,7 +4974,7 @@
       <c r="C4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="4" t="s">

</xml_diff>